<commit_message>
BBB spreadsheet cleanup results
</commit_message>
<xml_diff>
--- a/results/11-2021/11-2021_comparison_deflators.xlsx
+++ b/results/11-2021/11-2021_comparison_deflators.xlsx
@@ -650,31 +650,31 @@
         <v>-0.039</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.3141</v>
+        <v>-0.2535</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2084</v>
+        <v>-0.209</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.0851</v>
+        <v>-0.0857</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.1989</v>
+        <v>-0.1995</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.1534</v>
+        <v>-0.0735</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.099</v>
+        <v>-0.1004</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.5229</v>
+        <v>-0.5243</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.2671</v>
+        <v>-0.2685</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.1609</v>
+        <v>-0.1031</v>
       </c>
     </row>
     <row r="6">
@@ -735,10 +735,10 @@
         <v>-0.1267</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.0418</v>
+        <v>-0.0428</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0544</v>
+        <v>0.0535</v>
       </c>
       <c r="H7" t="n">
         <v>-0.0828</v>
@@ -747,10 +747,10 @@
         <v>-0.1407</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.1542</v>
+        <v>-0.1533</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.2003</v>
+        <v>-0.1994</v>
       </c>
       <c r="L7" t="n">
         <v>-0.0724</v>
@@ -808,37 +808,37 @@
         <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0226</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0448</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0061</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.003</v>
+        <v>-0.0295</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.0062</v>
+        <v>-0.0212</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.1304</v>
+        <v>-0.0212</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.0761</v>
+        <v>-0.0525</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.0439</v>
+        <v>-0.0401</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0498</v>
+        <v>-0.0396</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0213</v>
+        <v>-0.0248</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0314</v>
+        <v>-0.0244</v>
       </c>
     </row>
     <row r="10">
@@ -849,37 +849,37 @@
         <v>14</v>
       </c>
       <c r="C10" t="n">
-        <v>0.194</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4519</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0944</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1107</v>
+        <v>-0.0027</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0547</v>
+        <v>-0.005</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.0496</v>
+        <v>-0.0072</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.1522</v>
+        <v>-0.2309</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.0842</v>
+        <v>-0.1947</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.1234</v>
+        <v>-0.1809</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.154</v>
+        <v>-0.1675</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.0847</v>
+        <v>-0.125</v>
       </c>
     </row>
     <row r="11">
@@ -930,38 +930,32 @@
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="n">
-        <v>-0.3469</v>
-      </c>
-      <c r="D12" t="n">
-        <v>-0.0562</v>
-      </c>
-      <c r="E12" t="n">
-        <v>-0.0535</v>
-      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
       <c r="F12" t="n">
-        <v>-0.2471</v>
+        <v>-0.6014</v>
       </c>
       <c r="G12" t="n">
-        <v>0.7385</v>
+        <v>-0.6539</v>
       </c>
       <c r="H12" t="n">
-        <v>0.271</v>
+        <v>-0.8608</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2848</v>
+        <v>-0.6834</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.4164</v>
+        <v>0.0193</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.3931</v>
+        <v>0.0347</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.2219</v>
+        <v>0.1981</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.2025</v>
+        <v>0.0738</v>
       </c>
     </row>
     <row r="13">
@@ -978,31 +972,31 @@
         <v>0.2321</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1389</v>
+        <v>-0.1236</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.1073</v>
+        <v>-0.1112</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.1219</v>
+        <v>-0.1281</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.1116</v>
+        <v>-0.1171</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.0509</v>
+        <v>-0.0491</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.0428</v>
+        <v>-0.0434</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.6116</v>
+        <v>-0.6121</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.646</v>
+        <v>-0.6467</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.303</v>
+        <v>-0.3035</v>
       </c>
     </row>
     <row r="14">
@@ -1053,38 +1047,32 @@
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="n">
-        <v>-2.3436</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-2.1682</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-2.7222</v>
-      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
       <c r="F15" t="n">
-        <v>-1.5425</v>
+        <v>-2.0325</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.7782</v>
+        <v>-4.2436</v>
       </c>
       <c r="H15" t="n">
-        <v>-1.9507</v>
+        <v>-2.9287</v>
       </c>
       <c r="I15" t="n">
-        <v>-1.3203</v>
+        <v>-2.2538</v>
       </c>
       <c r="J15" t="n">
-        <v>-2.205</v>
+        <v>-1.8699</v>
       </c>
       <c r="K15" t="n">
-        <v>-3.3709</v>
+        <v>-2.9846</v>
       </c>
       <c r="L15" t="n">
-        <v>-1.649</v>
+        <v>-1.2404</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.9288</v>
+        <v>-0.621</v>
       </c>
     </row>
     <row r="16">
@@ -1347,31 +1335,31 @@
         <v>-0.0285</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.036</v>
+        <v>-0.0269</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.0281</v>
+        <v>-0.0195</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.0288</v>
+        <v>-0.0203</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.0281</v>
+        <v>-0.0198</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.0278</v>
+        <v>-0.0196</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.0298</v>
+        <v>-0.0219</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0306</v>
+        <v>-0.0229</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.0219</v>
+        <v>-0.0144</v>
       </c>
       <c r="M22" t="n">
-        <v>-0.0203</v>
+        <v>-0.0129</v>
       </c>
     </row>
     <row r="23">
@@ -1391,10 +1379,10 @@
         <v>0.1152</v>
       </c>
       <c r="F23" t="n">
-        <v>0.048</v>
+        <v>0.0489</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.0297</v>
+        <v>-0.0288</v>
       </c>
       <c r="H23" t="n">
         <v>0.1174</v>
@@ -1403,10 +1391,10 @@
         <v>0.0996</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0967</v>
+        <v>0.0957</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0727</v>
+        <v>0.0718</v>
       </c>
       <c r="L23" t="n">
         <v>-0.074</v>
@@ -1511,31 +1499,31 @@
         <v>157.4</v>
       </c>
       <c r="E26" t="n">
-        <v>159.2929</v>
+        <v>159.2979</v>
       </c>
       <c r="F26" t="n">
-        <v>161.2086</v>
+        <v>161.2187</v>
       </c>
       <c r="G26" t="n">
-        <v>163.1473</v>
+        <v>163.1626</v>
       </c>
       <c r="H26" t="n">
-        <v>165.1093</v>
+        <v>165.13</v>
       </c>
       <c r="I26" t="n">
-        <v>167.0949</v>
+        <v>167.1211</v>
       </c>
       <c r="J26" t="n">
-        <v>169.1044</v>
+        <v>169.1363</v>
       </c>
       <c r="K26" t="n">
-        <v>171.1381</v>
+        <v>171.1757</v>
       </c>
       <c r="L26" t="n">
-        <v>173.1962</v>
+        <v>173.2397</v>
       </c>
       <c r="M26" t="n">
-        <v>175.2791</v>
+        <v>175.3286</v>
       </c>
     </row>
     <row r="27">
@@ -1757,31 +1745,31 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.105</v>
+        <v>-0.0444</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.106</v>
+        <v>-0.1066</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.108</v>
+        <v>-0.1086</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.1104</v>
+        <v>-0.111</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.1132</v>
+        <v>-0.0333</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.1163</v>
+        <v>-0.1177</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.1196</v>
+        <v>-0.121</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.123</v>
+        <v>-0.1244</v>
       </c>
       <c r="M32" t="n">
-        <v>-0.1267</v>
+        <v>-0.0689</v>
       </c>
     </row>
     <row r="33">
@@ -1842,22 +1830,22 @@
         <v>0.0002</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.0699</v>
+        <v>-0.0708</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.0688</v>
+        <v>-0.0697</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0021</v>
+        <v>0.0022</v>
       </c>
       <c r="I34" t="n">
         <v>-0.0284</v>
       </c>
       <c r="J34" t="n">
-        <v>0.008</v>
+        <v>0.0089</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.0215</v>
+        <v>-0.0206</v>
       </c>
       <c r="L34" t="n">
         <v>-0.1174</v>
@@ -1915,37 +1903,37 @@
         <v>41</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>0.0226</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>-0.0448</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>-0.0061</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>-0.0265</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>-0.0149</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>0.1092</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>0.0235</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>0.0038</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>0.0102</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>-0.0035</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="37">
@@ -1956,37 +1944,37 @@
         <v>41</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0709</v>
+        <v>-0.1231</v>
       </c>
       <c r="D37" t="n">
-        <v>0.3138</v>
+        <v>-0.1382</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.152</v>
+        <v>-0.2464</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.1014</v>
+        <v>-0.2147</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.1102</v>
+        <v>-0.1699</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.1719</v>
+        <v>-0.1295</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.0084</v>
+        <v>-0.0871</v>
       </c>
       <c r="J37" t="n">
-        <v>0.0522</v>
+        <v>-0.0582</v>
       </c>
       <c r="K37" t="n">
-        <v>0.0229</v>
+        <v>-0.0346</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.0087</v>
+        <v>-0.0222</v>
       </c>
       <c r="M37" t="n">
-        <v>0.0403</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2037,38 +2025,32 @@
       <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C39" t="n">
-        <v>-0.1785</v>
-      </c>
-      <c r="D39" t="n">
-        <v>-0.0886</v>
-      </c>
-      <c r="E39" t="n">
-        <v>-0.5265</v>
-      </c>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
       <c r="F39" t="n">
-        <v>0.7039</v>
+        <v>0.3496</v>
       </c>
       <c r="G39" t="n">
-        <v>0.8767</v>
+        <v>-0.5157</v>
       </c>
       <c r="H39" t="n">
-        <v>1.2127</v>
+        <v>0.0809</v>
       </c>
       <c r="I39" t="n">
-        <v>1.1886</v>
+        <v>0.2205</v>
       </c>
       <c r="J39" t="n">
-        <v>-0.2198</v>
+        <v>0.216</v>
       </c>
       <c r="K39" t="n">
-        <v>-0.2159</v>
+        <v>0.2119</v>
       </c>
       <c r="L39" t="n">
-        <v>-0.2121</v>
+        <v>0.2079</v>
       </c>
       <c r="M39" t="n">
-        <v>-0.2084</v>
+        <v>0.068</v>
       </c>
     </row>
     <row r="40">
@@ -2085,31 +2067,31 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0231</v>
+        <v>0.0384</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0358</v>
+        <v>0.032</v>
       </c>
       <c r="G40" t="n">
-        <v>0.0357</v>
+        <v>0.0294</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0326</v>
+        <v>0.0271</v>
       </c>
       <c r="I40" t="n">
-        <v>-0.0129</v>
+        <v>-0.0111</v>
       </c>
       <c r="J40" t="n">
-        <v>-0.0054</v>
+        <v>-0.006</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.0039</v>
+        <v>-0.0043</v>
       </c>
       <c r="L40" t="n">
-        <v>-0.002</v>
+        <v>-0.0027</v>
       </c>
       <c r="M40" t="n">
-        <v>-0.0022</v>
+        <v>-0.0026</v>
       </c>
     </row>
     <row r="41">
@@ -2160,38 +2142,32 @@
       <c r="B42" t="s">
         <v>41</v>
       </c>
-      <c r="C42" t="n">
-        <v>-0.1076</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0.2252</v>
-      </c>
-      <c r="E42" t="n">
-        <v>-0.7338</v>
-      </c>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
       <c r="F42" t="n">
-        <v>0.4056</v>
+        <v>-0.0844</v>
       </c>
       <c r="G42" t="n">
-        <v>0.5325</v>
+        <v>-0.9329</v>
       </c>
       <c r="H42" t="n">
-        <v>0.8088</v>
+        <v>-0.1691</v>
       </c>
       <c r="I42" t="n">
-        <v>0.9655</v>
+        <v>0.0321</v>
       </c>
       <c r="J42" t="n">
-        <v>-0.3254</v>
+        <v>0.0097</v>
       </c>
       <c r="K42" t="n">
-        <v>-0.3734</v>
+        <v>0.013</v>
       </c>
       <c r="L42" t="n">
-        <v>-0.415</v>
+        <v>-0.0064</v>
       </c>
       <c r="M42" t="n">
-        <v>-0.4139</v>
+        <v>-0.1061</v>
       </c>
     </row>
     <row r="43">
@@ -2454,31 +2430,31 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>-0.0091</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>-0.0086</v>
+        <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.0085</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>-0.0083</v>
+        <v>0</v>
       </c>
       <c r="I49" t="n">
-        <v>-0.0081</v>
+        <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>-0.0079</v>
+        <v>0</v>
       </c>
       <c r="K49" t="n">
-        <v>-0.0077</v>
+        <v>0</v>
       </c>
       <c r="L49" t="n">
-        <v>-0.0075</v>
+        <v>0</v>
       </c>
       <c r="M49" t="n">
-        <v>-0.0074</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2498,22 +2474,22 @@
         <v>0.0001</v>
       </c>
       <c r="F50" t="n">
-        <v>0.0704</v>
+        <v>0.0714</v>
       </c>
       <c r="G50" t="n">
-        <v>0.0696</v>
+        <v>0.0705</v>
       </c>
       <c r="H50" t="n">
         <v>-0.0011</v>
       </c>
       <c r="I50" t="n">
-        <v>-0.0169</v>
+        <v>-0.017</v>
       </c>
       <c r="J50" t="n">
-        <v>-0.098</v>
+        <v>-0.0989</v>
       </c>
       <c r="K50" t="n">
-        <v>-0.1115</v>
+        <v>-0.1124</v>
       </c>
       <c r="L50" t="n">
         <v>-0.0571</v>
@@ -2618,31 +2594,31 @@
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>-0.005</v>
+        <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>-0.0101</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>-0.0154</v>
+        <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>-0.0207</v>
+        <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>-0.0262</v>
+        <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>-0.0318</v>
+        <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>-0.0376</v>
+        <v>0</v>
       </c>
       <c r="L53" t="n">
-        <v>-0.0435</v>
+        <v>0</v>
       </c>
       <c r="M53" t="n">
-        <v>-0.0495</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">

</xml_diff>

<commit_message>
BBB spreadsheet cleanup results (for real)
</commit_message>
<xml_diff>
--- a/results/11-2021/11-2021_comparison_deflators.xlsx
+++ b/results/11-2021/11-2021_comparison_deflators.xlsx
@@ -808,37 +808,37 @@
         <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>-0.0224</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.0448</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.0063</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0295</v>
+        <v>-0.003</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.0212</v>
+        <v>-0.0062</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.0212</v>
+        <v>-0.1304</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.0525</v>
+        <v>-0.0761</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.0401</v>
+        <v>-0.0439</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0396</v>
+        <v>-0.0496</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0248</v>
+        <v>-0.0213</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0244</v>
+        <v>-0.0314</v>
       </c>
     </row>
     <row r="10">
@@ -849,34 +849,34 @@
         <v>14</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.1231</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.1382</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.2464</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.0027</v>
+        <v>0.2121</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.005</v>
+        <v>0.1649</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.0072</v>
+        <v>0.1224</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.2309</v>
+        <v>-0.1438</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.1947</v>
+        <v>-0.1364</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.1809</v>
+        <v>-0.1463</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.1675</v>
+        <v>-0.1453</v>
       </c>
       <c r="M10" t="n">
         <v>-0.125</v>
@@ -930,17 +930,23 @@
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
+      <c r="C12" t="n">
+        <v>-0.1684</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0324</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.638</v>
+      </c>
       <c r="F12" t="n">
-        <v>-0.6014</v>
+        <v>-0.7926</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.6539</v>
+        <v>0.0168</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.8608</v>
+        <v>-0.7905</v>
       </c>
       <c r="I12" t="n">
         <v>-0.6834</v>
@@ -1047,32 +1053,38 @@
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
+      <c r="C15" t="n">
+        <v>-2.2358</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-2.3933</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-1.7935</v>
+      </c>
       <c r="F15" t="n">
-        <v>-2.0325</v>
+        <v>-1.9824</v>
       </c>
       <c r="G15" t="n">
-        <v>-4.2436</v>
+        <v>-3.3881</v>
       </c>
       <c r="H15" t="n">
-        <v>-2.9287</v>
+        <v>-2.838</v>
       </c>
       <c r="I15" t="n">
-        <v>-2.2538</v>
+        <v>-2.1902</v>
       </c>
       <c r="J15" t="n">
-        <v>-1.8699</v>
+        <v>-1.8154</v>
       </c>
       <c r="K15" t="n">
-        <v>-2.9846</v>
+        <v>-2.96</v>
       </c>
       <c r="L15" t="n">
-        <v>-1.2404</v>
+        <v>-1.2147</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.621</v>
+        <v>-0.628</v>
       </c>
     </row>
     <row r="16">
@@ -1903,37 +1915,37 @@
         <v>41</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0226</v>
+        <v>0.0002</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.0448</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.0061</v>
+        <v>0.0002</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.0265</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.0149</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0.1092</v>
+        <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0235</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>0.0038</v>
+        <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0102</v>
+        <v>0.0002</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.0035</v>
+        <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>0.007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1944,34 +1956,34 @@
         <v>41</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.1231</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.1382</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.2464</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.2147</v>
+        <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.1699</v>
+        <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.1295</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.0871</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.0582</v>
+        <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.0346</v>
+        <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.0222</v>
+        <v>0</v>
       </c>
       <c r="M37" t="n">
         <v>0</v>
@@ -2025,17 +2037,23 @@
       <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.165</v>
+      </c>
       <c r="F39" t="n">
-        <v>0.3496</v>
+        <v>0.1584</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.5157</v>
+        <v>0.1549</v>
       </c>
       <c r="H39" t="n">
-        <v>0.0809</v>
+        <v>0.1512</v>
       </c>
       <c r="I39" t="n">
         <v>0.2205</v>
@@ -2142,32 +2160,38 @@
       <c r="B42" t="s">
         <v>41</v>
       </c>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
+      <c r="C42" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.1949</v>
+      </c>
       <c r="F42" t="n">
-        <v>-0.0844</v>
+        <v>-0.0343</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.9329</v>
+        <v>-0.0773</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.1691</v>
+        <v>-0.0785</v>
       </c>
       <c r="I42" t="n">
-        <v>0.0321</v>
+        <v>0.0957</v>
       </c>
       <c r="J42" t="n">
-        <v>0.0097</v>
+        <v>0.0641</v>
       </c>
       <c r="K42" t="n">
-        <v>0.013</v>
+        <v>0.0376</v>
       </c>
       <c r="L42" t="n">
-        <v>-0.0064</v>
+        <v>0.0193</v>
       </c>
       <c r="M42" t="n">
-        <v>-0.1061</v>
+        <v>-0.1131</v>
       </c>
     </row>
     <row r="43">

</xml_diff>

<commit_message>
Incorporate Q3 revision and adjust based on MPI
</commit_message>
<xml_diff>
--- a/results/11-2021/11-2021_comparison_deflators.xlsx
+++ b/results/11-2021/11-2021_comparison_deflators.xlsx
@@ -650,10 +650,10 @@
         <v>-0.0648</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.2534</v>
+        <v>-0.2132</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.209</v>
+        <v>-0.2486</v>
       </c>
       <c r="G5" t="n">
         <v>-0.0856</v>
@@ -814,22 +814,22 @@
         <v>0.0448</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0062</v>
+        <v>0.0203</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.003</v>
+        <v>-0.007</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.0062</v>
+        <v>-0.0063</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.1304</v>
+        <v>-0.1352</v>
       </c>
       <c r="I9" t="n">
         <v>-0.0761</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.0439</v>
+        <v>-0.044</v>
       </c>
       <c r="K9" t="n">
         <v>-0.0496</v>
@@ -838,7 +838,7 @@
         <v>-0.0213</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0314</v>
+        <v>-0.0315</v>
       </c>
     </row>
     <row r="10">
@@ -937,25 +937,25 @@
         <v>0.0141</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6374</v>
+        <v>0.5054</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.7929</v>
+        <v>-0.7273</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0164</v>
+        <v>0.0803</v>
       </c>
       <c r="H12" t="n">
         <v>-0.7739</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.6834</v>
+        <v>-0.5601</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0193</v>
+        <v>-0.0431</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0346</v>
+        <v>-0.0266</v>
       </c>
       <c r="L12" t="n">
         <v>0.1981</v>
@@ -978,19 +978,19 @@
         <v>0.232</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1235</v>
+        <v>-0.1205</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.1112</v>
+        <v>-0.1116</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.1282</v>
+        <v>-0.1283</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.1171</v>
+        <v>-0.1173</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.0491</v>
+        <v>-0.0493</v>
       </c>
       <c r="J13" t="n">
         <v>-0.0435</v>
@@ -1002,7 +1002,7 @@
         <v>-0.6467</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.3035</v>
+        <v>-0.3036</v>
       </c>
     </row>
     <row r="14">
@@ -1060,31 +1060,31 @@
         <v>-2.2904</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.6637</v>
+        <v>-1.7426</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.841</v>
+        <v>-1.7903</v>
       </c>
       <c r="G15" t="n">
-        <v>-3.2558</v>
+        <v>-3.227</v>
       </c>
       <c r="H15" t="n">
-        <v>-2.8623</v>
+        <v>-2.8697</v>
       </c>
       <c r="I15" t="n">
-        <v>-2.2348</v>
+        <v>-2.1116</v>
       </c>
       <c r="J15" t="n">
-        <v>-1.8633</v>
+        <v>-1.9137</v>
       </c>
       <c r="K15" t="n">
-        <v>-2.9818</v>
+        <v>-3.0431</v>
       </c>
       <c r="L15" t="n">
         <v>-1.2245</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.6394</v>
+        <v>-0.6396</v>
       </c>
     </row>
     <row r="16">
@@ -1142,10 +1142,10 @@
         <v>0.418</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.244</v>
+        <v>-0.2039</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.142</v>
+        <v>-0.1816</v>
       </c>
       <c r="G17" t="n">
         <v>0.1377</v>
@@ -1224,25 +1224,25 @@
         <v>-0.0489</v>
       </c>
       <c r="E19" t="n">
-        <v>-1.2108</v>
+        <v>-1.1747</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0118</v>
+        <v>0.0014</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0013</v>
+        <v>-0.0335</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.033</v>
+        <v>-0.0353</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.035</v>
+        <v>-0.0348</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.0345</v>
+        <v>-0.0224</v>
       </c>
       <c r="K19" t="n">
-        <v>-1.0899</v>
+        <v>-1.0898</v>
       </c>
       <c r="L19" t="n">
         <v>-0.0002</v>
@@ -1306,10 +1306,10 @@
         <v>-0.1273</v>
       </c>
       <c r="E21" t="n">
-        <v>0.7575</v>
+        <v>0.7173</v>
       </c>
       <c r="F21" t="n">
-        <v>0.5123</v>
+        <v>0.552</v>
       </c>
       <c r="G21" t="n">
         <v>0.1133</v>
@@ -1757,10 +1757,10 @@
         <v>-0.0258</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.0442</v>
+        <v>-0.0041</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.1066</v>
+        <v>-0.1463</v>
       </c>
       <c r="G32" t="n">
         <v>-0.1086</v>
@@ -1921,16 +1921,16 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0.0002</v>
+        <v>0.0142</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>-0.004</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>-0.0048</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -1939,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
       <c r="L36" t="n">
         <v>0</v>
@@ -2044,25 +2044,25 @@
         <v>-0.0182</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1644</v>
+        <v>0.0325</v>
       </c>
       <c r="F39" t="n">
-        <v>0.1581</v>
+        <v>0.2237</v>
       </c>
       <c r="G39" t="n">
-        <v>0.1546</v>
+        <v>0.2185</v>
       </c>
       <c r="H39" t="n">
-        <v>0.1678</v>
+        <v>0.1677</v>
       </c>
       <c r="I39" t="n">
-        <v>0.2204</v>
+        <v>0.3438</v>
       </c>
       <c r="J39" t="n">
-        <v>0.2159</v>
+        <v>0.1536</v>
       </c>
       <c r="K39" t="n">
-        <v>0.2118</v>
+        <v>0.1506</v>
       </c>
       <c r="L39" t="n">
         <v>0.2079</v>
@@ -2085,31 +2085,31 @@
         <v>-0.0001</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0385</v>
+        <v>0.0415</v>
       </c>
       <c r="F40" t="n">
-        <v>0.032</v>
+        <v>0.0315</v>
       </c>
       <c r="G40" t="n">
-        <v>0.0294</v>
+        <v>0.0293</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0271</v>
+        <v>0.0269</v>
       </c>
       <c r="I40" t="n">
-        <v>-0.0111</v>
+        <v>-0.0112</v>
       </c>
       <c r="J40" t="n">
-        <v>-0.006</v>
+        <v>-0.0061</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.0043</v>
+        <v>-0.0044</v>
       </c>
       <c r="L40" t="n">
         <v>-0.0027</v>
       </c>
       <c r="M40" t="n">
-        <v>-0.0026</v>
+        <v>-0.0028</v>
       </c>
     </row>
     <row r="41">
@@ -2167,31 +2167,31 @@
         <v>0.1029</v>
       </c>
       <c r="E42" t="n">
-        <v>0.3247</v>
+        <v>0.2458</v>
       </c>
       <c r="F42" t="n">
-        <v>0.1071</v>
+        <v>0.1578</v>
       </c>
       <c r="G42" t="n">
-        <v>0.055</v>
+        <v>0.0838</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.1028</v>
+        <v>-0.1102</v>
       </c>
       <c r="I42" t="n">
-        <v>0.051</v>
+        <v>0.1743</v>
       </c>
       <c r="J42" t="n">
-        <v>0.0162</v>
+        <v>-0.0341</v>
       </c>
       <c r="K42" t="n">
-        <v>0.0158</v>
+        <v>-0.0455</v>
       </c>
       <c r="L42" t="n">
         <v>0.0095</v>
       </c>
       <c r="M42" t="n">
-        <v>-0.1245</v>
+        <v>-0.1247</v>
       </c>
     </row>
     <row r="43">
@@ -2249,10 +2249,10 @@
         <v>-0.0143</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.1048</v>
+        <v>-0.0647</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.106</v>
+        <v>-0.1457</v>
       </c>
       <c r="G44" t="n">
         <v>-0.108</v>
@@ -2331,22 +2331,22 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0.0007</v>
+        <v>0.0368</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>-0.0104</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>-0.0348</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>-0.0023</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>0.0121</v>
       </c>
       <c r="K46" t="n">
         <v>0</v>
@@ -2413,10 +2413,10 @@
         <v>0.0498</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1059</v>
+        <v>0.0658</v>
       </c>
       <c r="F48" t="n">
-        <v>0.107</v>
+        <v>0.1467</v>
       </c>
       <c r="G48" t="n">
         <v>0.1087</v>

</xml_diff>